<commit_message>
editing concentrations tab methods
</commit_message>
<xml_diff>
--- a/sheets/input/Arnot_match _alt_input.xlsx
+++ b/sheets/input/Arnot_match _alt_input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sample_and_Time_Input" sheetId="1" state="visible" r:id="rId2"/>
@@ -221,7 +221,7 @@
     <t xml:space="preserve">Disequilbrium factor of Particulate Organic Carbon (ony if Cwdo is unavaliable)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Beta Lipid Omn (default = 1)</t>
+    <t xml:space="preserve">Beta Lipid OM (default = 1)</t>
   </si>
   <si>
     <t xml:space="preserve">Beta Non-lipid OM (defualt = 0.035)</t>
@@ -1146,9 +1146,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1019160</xdr:colOff>
+      <xdr:colOff>1018800</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>189720</xdr:rowOff>
+      <xdr:rowOff>189360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1158,7 +1158,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14044680" y="863280"/>
-          <a:ext cx="9471600" cy="7619400"/>
+          <a:ext cx="9471240" cy="7619040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1625,9 +1625,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>3631320</xdr:colOff>
+      <xdr:colOff>3630960</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>183240</xdr:rowOff>
+      <xdr:rowOff>182880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1636,8 +1636,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12524400" y="699480"/>
-          <a:ext cx="3084840" cy="996120"/>
+          <a:off x="12525120" y="699480"/>
+          <a:ext cx="3084480" cy="995760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1724,7 +1724,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11809800" y="292320"/>
+          <a:off x="11810520" y="292320"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1769,7 +1769,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11809800" y="279360"/>
+          <a:off x="11810520" y="279360"/>
           <a:ext cx="0" cy="2071080"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1814,7 +1814,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11809800" y="2363400"/>
+          <a:off x="11810520" y="2363400"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1848,9 +1848,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2331720</xdr:colOff>
+      <xdr:colOff>2331360</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>189720</xdr:rowOff>
+      <xdr:rowOff>189360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1863,8 +1863,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16675560" y="10278720"/>
-          <a:ext cx="2331720" cy="735840"/>
+          <a:off x="16676280" y="10278720"/>
+          <a:ext cx="2331360" cy="735480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1885,9 +1885,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>4593240</xdr:colOff>
+      <xdr:colOff>4592880</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>87840</xdr:rowOff>
+      <xdr:rowOff>87480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1896,8 +1896,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11824920" y="2007000"/>
-          <a:ext cx="9443880" cy="3201480"/>
+          <a:off x="11825640" y="2007000"/>
+          <a:ext cx="9443520" cy="3201120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2364,9 +2364,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>786600</xdr:colOff>
+      <xdr:colOff>786240</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>190080</xdr:rowOff>
+      <xdr:rowOff>189720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2376,7 +2376,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16928640" y="190440"/>
-          <a:ext cx="3603600" cy="761400"/>
+          <a:ext cx="3603240" cy="761040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2506,9 +2506,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1133280</xdr:colOff>
+      <xdr:colOff>1132920</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>189720</xdr:rowOff>
+      <xdr:rowOff>189360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2518,7 +2518,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14774760" y="1714680"/>
-          <a:ext cx="2931120" cy="761040"/>
+          <a:ext cx="2930760" cy="760680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2590,9 +2590,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>644040</xdr:colOff>
+      <xdr:colOff>643680</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>133200</xdr:rowOff>
+      <xdr:rowOff>132840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2602,7 +2602,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10537200" y="2522160"/>
-          <a:ext cx="9088560" cy="3568320"/>
+          <a:ext cx="9088200" cy="3567960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3130,9 +3130,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>151560</xdr:colOff>
+      <xdr:colOff>151200</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
+      <xdr:rowOff>10080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3142,7 +3142,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10606320" y="674280"/>
-          <a:ext cx="4075920" cy="949680"/>
+          <a:ext cx="4075560" cy="949320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3249,9 +3249,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3566880</xdr:colOff>
+      <xdr:colOff>3566520</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>46800</xdr:rowOff>
+      <xdr:rowOff>46440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3261,7 +3261,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4629240" y="4925160"/>
-          <a:ext cx="5158440" cy="761400"/>
+          <a:ext cx="5158080" cy="761040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3363,9 +3363,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2593440</xdr:colOff>
+      <xdr:colOff>2593080</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>190440</xdr:rowOff>
+      <xdr:rowOff>190080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3375,7 +3375,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16049880" y="5488560"/>
-          <a:ext cx="4331520" cy="341640"/>
+          <a:ext cx="4331160" cy="341280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3447,9 +3447,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>5384160</xdr:colOff>
+      <xdr:colOff>5383800</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>138960</xdr:rowOff>
+      <xdr:rowOff>138600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3459,7 +3459,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9213840" y="76320"/>
-          <a:ext cx="5257080" cy="1497600"/>
+          <a:ext cx="5256720" cy="1497240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3661,9 +3661,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>6884640</xdr:colOff>
+      <xdr:colOff>6884280</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>88200</xdr:rowOff>
+      <xdr:rowOff>87840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3673,7 +3673,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10153440" y="2298600"/>
-          <a:ext cx="5817960" cy="659520"/>
+          <a:ext cx="5817600" cy="659160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3780,9 +3780,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>253440</xdr:colOff>
+      <xdr:colOff>253080</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>62640</xdr:rowOff>
+      <xdr:rowOff>62280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3792,7 +3792,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11960640" y="241200"/>
-          <a:ext cx="5136480" cy="392760"/>
+          <a:ext cx="5136120" cy="392400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3904,9 +3904,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>100800</xdr:colOff>
+      <xdr:colOff>100440</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>189720</xdr:rowOff>
+      <xdr:rowOff>189360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3916,7 +3916,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12062160" y="1295280"/>
-          <a:ext cx="3862800" cy="418320"/>
+          <a:ext cx="3862440" cy="417960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3973,9 +3973,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>469440</xdr:colOff>
+      <xdr:colOff>469080</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>189720</xdr:rowOff>
+      <xdr:rowOff>189360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3985,7 +3985,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12087720" y="2158560"/>
-          <a:ext cx="5225400" cy="698040"/>
+          <a:ext cx="5225040" cy="697680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4047,9 +4047,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>278640</xdr:colOff>
+      <xdr:colOff>278280</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>164520</xdr:rowOff>
+      <xdr:rowOff>164160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4059,7 +4059,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13899240" y="761760"/>
-          <a:ext cx="6531120" cy="5879520"/>
+          <a:ext cx="6530760" cy="5879160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4176,7 +4176,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="1" sqref="B6 B11"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4295,7 +4295,7 @@
   </sheetPr>
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -4619,7 +4619,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="B6 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4688,8 +4688,8 @@
   </sheetPr>
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="B6 A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4858,7 +4858,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="1" sqref="B6 B15"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4928,7 +4928,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H18" activeCellId="1" sqref="B6 H18"/>
+      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5315,7 +5315,7 @@
   <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="1" sqref="B6 B23"/>
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5563,7 +5563,7 @@
   <dimension ref="A1:AMJ4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G21" activeCellId="1" sqref="B6 G21"/>
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6137,7 +6137,7 @@
   <dimension ref="A1:AW100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="1" sqref="B6 C27"/>
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>